<commit_message>
added many pngs, cleaned up README a bit
</commit_message>
<xml_diff>
--- a/notebooks/plot_helius_results/helius_results.xlsx
+++ b/notebooks/plot_helius_results/helius_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryankuster/github/metagenome_abundances/notebooks/plot_helius_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302F7139-FED5-4F4F-9279-F24190A57726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD818D9F-AB96-DF40-860F-CED96D5D6E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{C1EA9467-7B57-6D48-A728-9EF515B76259}"/>
   </bookViews>
@@ -498,10 +498,10 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M21" sqref="M21"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1735,11 +1735,11 @@
         <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ecori_ecori</v>
+        <v>ecori_msei</v>
       </c>
       <c r="E19" s="1">
         <v>306</v>
@@ -1802,11 +1802,11 @@
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D20" s="1" t="str">
         <f t="shared" ref="D20" si="5">_xlfn.CONCAT(B20,"_",C20)</f>
-        <v>ecori_ecori</v>
+        <v>ecori_msei</v>
       </c>
       <c r="E20" s="1">
         <v>506</v>

</xml_diff>